<commit_message>
Added headers to code
</commit_message>
<xml_diff>
--- a/ProjectTemplate.xlsx
+++ b/ProjectTemplate.xlsx
@@ -6571,7 +6571,7 @@
   <dimension ref="J9:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6598,52 +6598,52 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="4102" r:id="rId3" name="BtnDbClass">
+        <control shapeId="4101" r:id="rId3" name="BtnGenCollection">
           <controlPr defaultSize="0" autoLine="0" r:id="rId4">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>6</xdr:col>
                 <xdr:colOff>57150</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>7</xdr:col>
                 <xdr:colOff>314325</xdr:colOff>
-                <xdr:row>9</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="4102" r:id="rId3" name="BtnDbClass"/>
+        <control shapeId="4101" r:id="rId3" name="BtnGenCollection"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="4097" r:id="rId5" name="BtmGenClass">
+        <control shapeId="4099" r:id="rId5" name="BtnGenerateProc">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>6</xdr:col>
                 <xdr:colOff>57150</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
+                <xdr:row>13</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>7</xdr:col>
                 <xdr:colOff>314325</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="4097" r:id="rId5" name="BtmGenClass"/>
+        <control shapeId="4099" r:id="rId5" name="BtnGenerateProc"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -6673,52 +6673,52 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="4099" r:id="rId9" name="BtnGenerateProc">
+        <control shapeId="4097" r:id="rId9" name="BtmGenClass">
           <controlPr defaultSize="0" autoLine="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>6</xdr:col>
                 <xdr:colOff>57150</xdr:colOff>
-                <xdr:row>13</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>7</xdr:col>
                 <xdr:colOff>314325</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="4099" r:id="rId9" name="BtnGenerateProc"/>
+        <control shapeId="4097" r:id="rId9" name="BtmGenClass"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="4101" r:id="rId11" name="BtnGenCollection">
+        <control shapeId="4102" r:id="rId11" name="BtnDbClass">
           <controlPr defaultSize="0" autoLine="0" r:id="rId12">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>6</xdr:col>
                 <xdr:colOff>57150</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>7</xdr:col>
                 <xdr:colOff>314325</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="4101" r:id="rId11" name="BtnGenCollection"/>
+        <control shapeId="4102" r:id="rId11" name="BtnDbClass"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>